<commit_message>
Updated OVWDemo Sheet for root pages.
</commit_message>
<xml_diff>
--- a/docs/OVW Sheets/OVWDemo_rroot.xlsx
+++ b/docs/OVW Sheets/OVWDemo_rroot.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OVW Migration Latest\OVWMigration\docs\OVW Sheets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9735" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="9735" firstSheet="37" activeTab="47"/>
   </bookViews>
   <sheets>
     <sheet name="de_de" sheetId="11" r:id="rId1"/>
@@ -71,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="94">
   <si>
     <t>products</t>
   </si>
@@ -347,6 +342,12 @@
   </si>
   <si>
     <t>http://www.cisco.com/web/ANZ/netsol/index.html</t>
+  </si>
+  <si>
+    <t>index-Rrootvar1</t>
+  </si>
+  <si>
+    <t>index-Rrootvar2</t>
   </si>
 </sst>
 </file>
@@ -700,7 +701,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -711,7 +712,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,8 +726,8 @@
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -736,8 +737,8 @@
       <c r="A2" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -771,8 +772,8 @@
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -782,8 +783,8 @@
       <c r="A2" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -818,8 +819,8 @@
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -829,8 +830,8 @@
       <c r="A2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -864,8 +865,8 @@
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -875,8 +876,8 @@
       <c r="A2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -910,8 +911,8 @@
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -921,8 +922,8 @@
       <c r="A2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -956,8 +957,8 @@
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -967,8 +968,8 @@
       <c r="A2" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1002,8 +1003,8 @@
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1013,8 +1014,8 @@
       <c r="A2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1048,8 +1049,8 @@
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1059,8 +1060,8 @@
       <c r="A2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1094,8 +1095,8 @@
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1105,8 +1106,8 @@
       <c r="A2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1140,8 +1141,8 @@
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1151,8 +1152,8 @@
       <c r="A2" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1186,8 +1187,8 @@
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1197,8 +1198,8 @@
       <c r="A2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1218,7 +1219,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,8 +1233,8 @@
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1243,8 +1244,8 @@
       <c r="A2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1264,7 +1265,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1278,11 +1279,11 @@
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
+      <c r="C1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1312,8 +1313,8 @@
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1323,8 +1324,8 @@
       <c r="A2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1358,8 +1359,8 @@
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1369,8 +1370,8 @@
       <c r="A2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1404,8 +1405,8 @@
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1415,8 +1416,8 @@
       <c r="A2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1450,8 +1451,8 @@
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1461,8 +1462,8 @@
       <c r="A2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1482,7 +1483,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,11 +1497,11 @@
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
+      <c r="C1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1516,7 +1517,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1530,11 +1531,11 @@
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
+      <c r="C1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1564,8 +1565,8 @@
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1575,8 +1576,8 @@
       <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1610,8 +1611,8 @@
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1621,8 +1622,8 @@
       <c r="A2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1642,7 +1643,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1656,11 +1657,11 @@
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
+      <c r="C1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1676,7 +1677,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1690,8 +1691,8 @@
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1701,8 +1702,8 @@
       <c r="A2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1736,8 +1737,8 @@
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1747,8 +1748,8 @@
       <c r="A2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1782,8 +1783,8 @@
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1793,8 +1794,8 @@
       <c r="A2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1828,8 +1829,8 @@
       <c r="A1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1839,8 +1840,8 @@
       <c r="A2" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1874,8 +1875,8 @@
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1885,8 +1886,8 @@
       <c r="A2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1920,8 +1921,8 @@
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1931,8 +1932,8 @@
       <c r="A2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1966,8 +1967,8 @@
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1977,8 +1978,8 @@
       <c r="A2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -2012,8 +2013,8 @@
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2023,8 +2024,8 @@
       <c r="A2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -2058,8 +2059,8 @@
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2069,8 +2070,8 @@
       <c r="A2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -2104,8 +2105,8 @@
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2115,8 +2116,8 @@
       <c r="A2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -2150,8 +2151,8 @@
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2161,8 +2162,8 @@
       <c r="A2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -2181,8 +2182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2196,8 +2197,8 @@
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2207,8 +2208,8 @@
       <c r="A2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -2228,7 +2229,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1"/>
+      <selection activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2242,11 +2243,11 @@
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
+      <c r="C1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2276,8 +2277,8 @@
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2287,8 +2288,8 @@
       <c r="A2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -2322,8 +2323,8 @@
       <c r="A1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2333,8 +2334,8 @@
       <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -2368,8 +2369,8 @@
       <c r="A1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2379,8 +2380,8 @@
       <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -2414,8 +2415,8 @@
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2425,8 +2426,8 @@
       <c r="A2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -2460,8 +2461,8 @@
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2471,8 +2472,8 @@
       <c r="A2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -2506,8 +2507,8 @@
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2517,8 +2518,8 @@
       <c r="A2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -2538,7 +2539,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="B1" sqref="B1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2552,8 +2553,8 @@
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2563,8 +2564,8 @@
       <c r="A2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -2583,8 +2584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2598,11 +2599,11 @@
       <c r="A1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
+      <c r="C1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2632,8 +2633,8 @@
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2643,8 +2644,8 @@
       <c r="A2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -2678,8 +2679,8 @@
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2689,8 +2690,8 @@
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -2724,8 +2725,8 @@
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2735,8 +2736,8 @@
       <c r="A2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -2770,8 +2771,8 @@
       <c r="A1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2781,8 +2782,8 @@
       <c r="A2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -2816,8 +2817,8 @@
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2827,8 +2828,8 @@
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>

</xml_diff>